<commit_message>
export -Initial Rating - Users
</commit_message>
<xml_diff>
--- a/filename.xlsx
+++ b/filename.xlsx
@@ -375,69 +375,741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:DS5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Product</v>
+        <v>User</v>
       </c>
       <c r="B1" t="str">
-        <v>Price</v>
+        <v>image 19</v>
       </c>
       <c r="C1" t="str">
-        <v>Quantity</v>
+        <v>image 20</v>
+      </c>
+      <c r="D1" t="str">
+        <v>image 21</v>
+      </c>
+      <c r="E1" t="str">
+        <v>image 22</v>
+      </c>
+      <c r="F1" t="str">
+        <v>image 23</v>
+      </c>
+      <c r="G1" t="str">
+        <v>image 24</v>
+      </c>
+      <c r="H1" t="str">
+        <v>image 25</v>
+      </c>
+      <c r="I1" t="str">
+        <v>image 26</v>
+      </c>
+      <c r="J1" t="str">
+        <v>image 27</v>
+      </c>
+      <c r="K1" t="str">
+        <v>image 28</v>
+      </c>
+      <c r="L1" t="str">
+        <v>image 29</v>
+      </c>
+      <c r="M1" t="str">
+        <v>image 30</v>
+      </c>
+      <c r="N1" t="str">
+        <v>image 31</v>
+      </c>
+      <c r="O1" t="str">
+        <v>image 32</v>
+      </c>
+      <c r="P1" t="str">
+        <v>image 33</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>image 34</v>
+      </c>
+      <c r="R1" t="str">
+        <v>image 35</v>
+      </c>
+      <c r="S1" t="str">
+        <v>image 36</v>
+      </c>
+      <c r="T1" t="str">
+        <v>image 37</v>
+      </c>
+      <c r="U1" t="str">
+        <v>image 38</v>
+      </c>
+      <c r="V1" t="str">
+        <v>image 39</v>
+      </c>
+      <c r="W1" t="str">
+        <v>image 40</v>
+      </c>
+      <c r="X1" t="str">
+        <v>image 41</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>image 42</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>image 43</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>image 44</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>image 45</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>image 46</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>image 47</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>image 48</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>image 49</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>image 50</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>image 51</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>image 52</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>image 53</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>image 54</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>image 55</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>image 56</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>image 57</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>image 58</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>image 59</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>image 60</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>image 61</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>image 62</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>image 63</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>image 64</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>image 65</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>image 66</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>image 67</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>image 68</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>image 69</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>image 70</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>image 71</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>image 72</v>
+      </c>
+      <c r="BD1" t="str">
+        <v>image 73</v>
+      </c>
+      <c r="BE1" t="str">
+        <v>image 74</v>
+      </c>
+      <c r="BF1" t="str">
+        <v>image 75</v>
+      </c>
+      <c r="BG1" t="str">
+        <v>image 76</v>
+      </c>
+      <c r="BH1" t="str">
+        <v>image 77</v>
+      </c>
+      <c r="BI1" t="str">
+        <v>image 78</v>
+      </c>
+      <c r="BJ1" t="str">
+        <v>image 79</v>
+      </c>
+      <c r="BK1" t="str">
+        <v>image 80</v>
+      </c>
+      <c r="BL1" t="str">
+        <v>image 81</v>
+      </c>
+      <c r="BM1" t="str">
+        <v>image 82</v>
+      </c>
+      <c r="BN1" t="str">
+        <v>image 83</v>
+      </c>
+      <c r="BO1" t="str">
+        <v>image 84</v>
+      </c>
+      <c r="BP1" t="str">
+        <v>image 85</v>
+      </c>
+      <c r="BQ1" t="str">
+        <v>image 86</v>
+      </c>
+      <c r="BR1" t="str">
+        <v>image 87</v>
+      </c>
+      <c r="BS1" t="str">
+        <v>image 88</v>
+      </c>
+      <c r="BT1" t="str">
+        <v>image 89</v>
+      </c>
+      <c r="BU1" t="str">
+        <v>image 90</v>
+      </c>
+      <c r="BV1" t="str">
+        <v>image 91</v>
+      </c>
+      <c r="BW1" t="str">
+        <v>image 92</v>
+      </c>
+      <c r="BX1" t="str">
+        <v>image 93</v>
+      </c>
+      <c r="BY1" t="str">
+        <v>image 94</v>
+      </c>
+      <c r="BZ1" t="str">
+        <v>image 95</v>
+      </c>
+      <c r="CA1" t="str">
+        <v>image 96</v>
+      </c>
+      <c r="CB1" t="str">
+        <v>image 97</v>
+      </c>
+      <c r="CC1" t="str">
+        <v>image 98</v>
+      </c>
+      <c r="CD1" t="str">
+        <v>image 99</v>
+      </c>
+      <c r="CE1" t="str">
+        <v>image 100</v>
+      </c>
+      <c r="CF1" t="str">
+        <v>image 101</v>
+      </c>
+      <c r="CG1" t="str">
+        <v>image 102</v>
+      </c>
+      <c r="CH1" t="str">
+        <v>image 103</v>
+      </c>
+      <c r="CI1" t="str">
+        <v>image 104</v>
+      </c>
+      <c r="CJ1" t="str">
+        <v>image 105</v>
+      </c>
+      <c r="CK1" t="str">
+        <v>image 106</v>
+      </c>
+      <c r="CL1" t="str">
+        <v>image 107</v>
+      </c>
+      <c r="CM1" t="str">
+        <v>image 108</v>
+      </c>
+      <c r="CN1" t="str">
+        <v>image 109</v>
+      </c>
+      <c r="CO1" t="str">
+        <v>image 110</v>
+      </c>
+      <c r="CP1" t="str">
+        <v>image 111</v>
+      </c>
+      <c r="CQ1" t="str">
+        <v>image 112</v>
+      </c>
+      <c r="CR1" t="str">
+        <v>image 113</v>
+      </c>
+      <c r="CS1" t="str">
+        <v>image 114</v>
+      </c>
+      <c r="CT1" t="str">
+        <v>image 115</v>
+      </c>
+      <c r="CU1" t="str">
+        <v>image 116</v>
+      </c>
+      <c r="CV1" t="str">
+        <v>image 117</v>
+      </c>
+      <c r="CW1" t="str">
+        <v>image 118</v>
+      </c>
+      <c r="CX1" t="str">
+        <v>image 119</v>
+      </c>
+      <c r="CY1" t="str">
+        <v>image 120</v>
+      </c>
+      <c r="CZ1" t="str">
+        <v>image 121</v>
+      </c>
+      <c r="DA1" t="str">
+        <v>image 122</v>
+      </c>
+      <c r="DB1" t="str">
+        <v>image 123</v>
+      </c>
+      <c r="DC1" t="str">
+        <v>image 124</v>
+      </c>
+      <c r="DD1" t="str">
+        <v>image 125</v>
+      </c>
+      <c r="DE1" t="str">
+        <v>image 126</v>
+      </c>
+      <c r="DF1" t="str">
+        <v>image 127</v>
+      </c>
+      <c r="DG1" t="str">
+        <v>image 128</v>
+      </c>
+      <c r="DH1" t="str">
+        <v>image 129</v>
+      </c>
+      <c r="DI1" t="str">
+        <v>image 130</v>
+      </c>
+      <c r="DJ1" t="str">
+        <v>image 131</v>
+      </c>
+      <c r="DK1" t="str">
+        <v>image 132</v>
+      </c>
+      <c r="DL1" t="str">
+        <v>image 133</v>
+      </c>
+      <c r="DM1" t="str">
+        <v>image 134</v>
+      </c>
+      <c r="DN1" t="str">
+        <v>image 135</v>
+      </c>
+      <c r="DO1" t="str">
+        <v>image 136</v>
+      </c>
+      <c r="DP1" t="str">
+        <v>image 137</v>
+      </c>
+      <c r="DQ1" t="str">
+        <v>image 138</v>
+      </c>
+      <c r="DR1" t="str">
+        <v>image 139</v>
+      </c>
+      <c r="DS1" t="str">
+        <v>image 140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Beverage</v>
-      </c>
-      <c r="B2" t="str">
-        <v>$ 10</v>
+        <v>lironoskar@gmail.com</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
       <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
         <v>2</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>8</v>
+      </c>
+      <c r="S2">
+        <v>8</v>
+      </c>
+      <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2">
+        <v>8</v>
+      </c>
+      <c r="V2">
+        <v>9</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>8</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>9</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
+        <v>8</v>
+      </c>
+      <c r="AD2">
+        <v>10</v>
+      </c>
+      <c r="AE2">
+        <v>9</v>
+      </c>
+      <c r="AF2">
+        <v>7</v>
+      </c>
+      <c r="AG2">
+        <v>10</v>
+      </c>
+      <c r="AH2">
+        <v>9</v>
+      </c>
+      <c r="AI2">
+        <v>9</v>
+      </c>
+      <c r="AJ2">
+        <v>10</v>
+      </c>
+      <c r="AK2">
+        <v>10</v>
+      </c>
+      <c r="AL2">
+        <v>10</v>
+      </c>
+      <c r="AN2">
+        <v>4</v>
+      </c>
+      <c r="AO2">
+        <v>10</v>
+      </c>
+      <c r="AP2">
+        <v>9</v>
+      </c>
+      <c r="AQ2">
+        <v>10</v>
+      </c>
+      <c r="AR2">
+        <v>10</v>
+      </c>
+      <c r="AS2">
+        <v>9</v>
+      </c>
+      <c r="AT2">
+        <v>8</v>
+      </c>
+      <c r="AU2">
+        <v>9</v>
+      </c>
+      <c r="AV2">
+        <v>9</v>
+      </c>
+      <c r="AW2">
+        <v>10</v>
+      </c>
+      <c r="AX2">
+        <v>9</v>
+      </c>
+      <c r="AY2">
+        <v>7</v>
+      </c>
+      <c r="AZ2">
+        <v>8</v>
+      </c>
+      <c r="BA2">
+        <v>9</v>
+      </c>
+      <c r="BB2">
+        <v>10</v>
+      </c>
+      <c r="BC2">
+        <v>6</v>
+      </c>
+      <c r="BD2">
+        <v>7</v>
+      </c>
+      <c r="BF2">
+        <v>5</v>
+      </c>
+      <c r="BG2">
+        <v>10</v>
+      </c>
+      <c r="BH2">
+        <v>3</v>
+      </c>
+      <c r="BI2">
+        <v>4</v>
+      </c>
+      <c r="BJ2">
+        <v>9</v>
+      </c>
+      <c r="BL2">
+        <v>10</v>
+      </c>
+      <c r="BM2">
+        <v>10</v>
+      </c>
+      <c r="BN2">
+        <v>10</v>
+      </c>
+      <c r="BO2">
+        <v>3</v>
+      </c>
+      <c r="BP2">
+        <v>8</v>
+      </c>
+      <c r="BQ2">
+        <v>5</v>
+      </c>
+      <c r="BR2">
+        <v>6</v>
+      </c>
+      <c r="BS2">
+        <v>9</v>
+      </c>
+      <c r="BT2">
+        <v>7</v>
+      </c>
+      <c r="BU2">
+        <v>7</v>
+      </c>
+      <c r="BW2">
+        <v>7</v>
+      </c>
+      <c r="BX2">
+        <v>7</v>
+      </c>
+      <c r="BY2">
+        <v>6</v>
+      </c>
+      <c r="BZ2">
+        <v>8</v>
+      </c>
+      <c r="CA2">
+        <v>7</v>
+      </c>
+      <c r="CC2">
+        <v>9</v>
+      </c>
+      <c r="CD2">
+        <v>10</v>
+      </c>
+      <c r="CE2">
+        <v>6</v>
+      </c>
+      <c r="CG2">
+        <v>8</v>
+      </c>
+      <c r="CH2">
+        <v>5</v>
+      </c>
+      <c r="CI2">
+        <v>9</v>
+      </c>
+      <c r="CJ2">
+        <v>6</v>
+      </c>
+      <c r="CK2">
+        <v>10</v>
+      </c>
+      <c r="CL2">
+        <v>5</v>
+      </c>
+      <c r="CN2">
+        <v>7</v>
+      </c>
+      <c r="CO2">
+        <v>9</v>
+      </c>
+      <c r="CP2">
+        <v>9</v>
+      </c>
+      <c r="CR2">
+        <v>10</v>
+      </c>
+      <c r="CT2">
+        <v>6</v>
+      </c>
+      <c r="CU2">
+        <v>8</v>
+      </c>
+      <c r="CW2">
+        <v>9</v>
+      </c>
+      <c r="CX2">
+        <v>9</v>
+      </c>
+      <c r="CY2">
+        <v>10</v>
+      </c>
+      <c r="CZ2">
+        <v>10</v>
+      </c>
+      <c r="DA2">
+        <v>8</v>
+      </c>
+      <c r="DC2">
+        <v>6</v>
+      </c>
+      <c r="DE2">
+        <v>8</v>
+      </c>
+      <c r="DF2">
+        <v>10</v>
+      </c>
+      <c r="DG2">
+        <v>6</v>
+      </c>
+      <c r="DH2">
+        <v>8</v>
+      </c>
+      <c r="DI2">
+        <v>10</v>
+      </c>
+      <c r="DK2">
+        <v>10</v>
+      </c>
+      <c r="DL2">
+        <v>1</v>
+      </c>
+      <c r="DM2">
+        <v>9</v>
+      </c>
+      <c r="DN2">
+        <v>9</v>
+      </c>
+      <c r="DO2">
+        <v>9</v>
+      </c>
+      <c r="DP2">
+        <v>9</v>
+      </c>
+      <c r="DQ2">
+        <v>10</v>
+      </c>
+      <c r="DR2">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Snack</v>
-      </c>
-      <c r="B3" t="str">
-        <v>$ 12</v>
-      </c>
-      <c r="C3">
+        <v>tali@gmail.com</v>
+      </c>
+      <c r="S3">
         <v>6</v>
+      </c>
+      <c r="AK3">
+        <v>7</v>
+      </c>
+      <c r="CK3">
+        <v>8</v>
+      </c>
+      <c r="CR3">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Beverage</v>
-      </c>
-      <c r="B4" t="str">
-        <v>$ 10</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+        <v>tali2@gmail.com</v>
+      </c>
+      <c r="AE4">
+        <v>7</v>
+      </c>
+      <c r="BX4">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Snack</v>
-      </c>
-      <c r="B5" t="str">
-        <v>$ 12</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>talii@gmail.com</v>
+      </c>
+      <c r="R5">
+        <v>9</v>
+      </c>
+      <c r="CR5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:DS5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>